<commit_message>
ttext - small updates
</commit_message>
<xml_diff>
--- a/TText/TText_testpop.xlsx
+++ b/TText/TText_testpop.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7919FA-C39A-48E3-9AF0-42852E231669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8EB30-C619-4B4F-A491-52046356966E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46188" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22428" yWindow="3156" windowWidth="23064" windowHeight="11256" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#TText test pop" sheetId="1" r:id="rId1"/>
@@ -883,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1211,7 +1211,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AE7184-86BE-4BBF-B79A-5AA702054FD3}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1538,7 +1540,10 @@
         <f>$A14</f>
         <v>Acc_TNO_ad</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="str">
+        <f>$A14</f>
+        <v>Acc_TNO_ad</v>
+      </c>
       <c r="C21" s="10" t="s">
         <v>106</v>
       </c>

</xml_diff>